<commit_message>
Add new code to analyze compliance data (also new).
</commit_message>
<xml_diff>
--- a/data/remote_sensing_monitor_evaluation.xlsx
+++ b/data/remote_sensing_monitor_evaluation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -17,6 +17,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="401">
   <si>
     <t>action-found</t>
   </si>
@@ -1102,6 +1105,132 @@
   </si>
   <si>
     <t>Not sure what water it's talking about</t>
+  </si>
+  <si>
+    <t>09-2009; 03-2011</t>
+  </si>
+  <si>
+    <t>11-2013; 04-2014; 09-2014</t>
+  </si>
+  <si>
+    <t>09-2008; 04-2010</t>
+  </si>
+  <si>
+    <t>Image quality before 2010 too poor</t>
+  </si>
+  <si>
+    <t>04-2011; 08-2012… 03-2015</t>
+  </si>
+  <si>
+    <t>10-2009; 03-2013</t>
+  </si>
+  <si>
+    <t>09-2009; 09-2010; 04-2011… 03-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Hard to discern area b/c road work goes on for miles</t>
+  </si>
+  <si>
+    <t>01-2011; 02-2014</t>
+  </si>
+  <si>
+    <t>12-2008; 12-2010… 04-2014</t>
+  </si>
+  <si>
+    <t>Area consists of 2 plots - 1 finished construction between 12-2010 and 01-2012. Other has not had any construction since being cleared</t>
+  </si>
+  <si>
+    <t>12-2005; 06-2009; 09-2010… 05-2014</t>
+  </si>
+  <si>
+    <t>Same project as: 43440-2010-F-0656 (row 40)</t>
+  </si>
+  <si>
+    <t>08-2013; 02-2014; 04-2014; 07-2014; 02-2015; 04-2015; 07-2015</t>
+  </si>
+  <si>
+    <t>12-2010; 02-2014</t>
+  </si>
+  <si>
+    <t>03-2010; 12-2010; 03-2011; 04-2012… 12-2014</t>
+  </si>
+  <si>
+    <t>Not sure about area b/c it goes on along the coast for miles. Does this count as natural --&gt; natural</t>
+  </si>
+  <si>
+    <t>08-2009; 07-2010; 12-2011… 10-2014</t>
+  </si>
+  <si>
+    <t>02-2014; 03-2015</t>
+  </si>
+  <si>
+    <t>05-2013; 10-2015</t>
+  </si>
+  <si>
+    <t>04-2013; 09-2013; 04-2014</t>
+  </si>
+  <si>
+    <t>12-2010; 06-2011; 10-2014; 05-2015</t>
+  </si>
+  <si>
+    <t>Doesn't look like any sand was added</t>
+  </si>
+  <si>
+    <t>07-2014; 04-2015; 07-2015</t>
+  </si>
+  <si>
+    <t>Along shore about 0.3 mi</t>
+  </si>
+  <si>
+    <t>07-2010; 09-2010… 03-2015</t>
+  </si>
+  <si>
+    <t>Stream covered by trees all along banks. Can't see any difference</t>
+  </si>
+  <si>
+    <t>05-2010; 12-2010; 01-2012… 02-2015</t>
+  </si>
+  <si>
+    <t>07-2012; 07-2014</t>
+  </si>
+  <si>
+    <t>08-2006; 03-2009; 03-2011… 10-2013</t>
+  </si>
+  <si>
+    <t>09-2011; 03-2013</t>
+  </si>
+  <si>
+    <t>Not sure how to categorize action found - 05-2010 pic clearly reveals burn area, and every pic after that shows green growth. Does that count? (see images)</t>
+  </si>
+  <si>
+    <t>Think I found the burn area, but it's 2.8 mi SW of pin. (see images)</t>
+  </si>
+  <si>
+    <t>Started FY 2014, but the title says "created Nov 2013"… does that mean the project or consultation? Not sure what I’m looking at in water (see images)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07-2011; 05-2013 </t>
+  </si>
+  <si>
+    <t>11-2007; 01-2008; 03-2009… 04-2014</t>
+  </si>
+  <si>
+    <t>03-2010; 05-2010; 06-2010; 09-2010… 04-2015</t>
+  </si>
+  <si>
+    <t>After picture is only 2 montsh after conclusion date</t>
+  </si>
+  <si>
+    <t>12-2009; 03-2010; 07-2010; 09-2010… 07-2011</t>
+  </si>
+  <si>
+    <t>06-2013; 02-2014; 03-2014… 10-2015</t>
+  </si>
+  <si>
+    <t>06-2009; 10-2011; 10-2011; 06-2012</t>
   </si>
 </sst>
 </file>
@@ -1502,10 +1631,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="347">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2132,8 +2262,8 @@
   <dimension ref="A1:L207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I147" sqref="I147"/>
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K189" sqref="K189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6221,21 +6351,44 @@
       <c r="A148" t="s">
         <v>277</v>
       </c>
+      <c r="B148">
+        <v>1</v>
+      </c>
       <c r="C148">
         <v>47.4773</v>
       </c>
       <c r="D148">
         <v>-124.03758000000001</v>
       </c>
-      <c r="G148" s="2"/>
-      <c r="H148" s="2"/>
-      <c r="J148" s="2"/>
-      <c r="K148" s="2"/>
+      <c r="E148">
+        <v>3</v>
+      </c>
+      <c r="F148">
+        <v>235</v>
+      </c>
+      <c r="G148" s="2">
+        <v>40603</v>
+      </c>
+      <c r="H148" s="2">
+        <v>40603</v>
+      </c>
+      <c r="I148">
+        <v>1</v>
+      </c>
+      <c r="J148" s="2">
+        <v>33025</v>
+      </c>
+      <c r="K148" s="2" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>278</v>
       </c>
+      <c r="B149">
+        <v>0</v>
+      </c>
       <c r="C149">
         <v>33.300020000000004</v>
       </c>
@@ -6244,13 +6397,20 @@
       </c>
       <c r="G149" s="2"/>
       <c r="H149" s="2"/>
-      <c r="J149" s="2"/>
-      <c r="K149" s="2"/>
+      <c r="J149" s="2">
+        <v>34455</v>
+      </c>
+      <c r="K149" s="2" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>279</v>
       </c>
+      <c r="B150">
+        <v>0</v>
+      </c>
       <c r="C150">
         <v>35.072229999999998</v>
       </c>
@@ -6259,71 +6419,159 @@
       </c>
       <c r="G150" s="2"/>
       <c r="H150" s="2"/>
-      <c r="J150" s="2"/>
-      <c r="K150" s="2"/>
+      <c r="J150" s="2">
+        <v>35490</v>
+      </c>
+      <c r="K150" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="L150" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>280</v>
       </c>
+      <c r="B151">
+        <v>1</v>
+      </c>
       <c r="C151">
         <v>47.500239999999998</v>
       </c>
       <c r="D151">
         <v>-124.05605</v>
       </c>
-      <c r="G151" s="2"/>
-      <c r="H151" s="2"/>
-      <c r="J151" s="2"/>
-      <c r="K151" s="2"/>
+      <c r="E151">
+        <v>3</v>
+      </c>
+      <c r="F151">
+        <v>46</v>
+      </c>
+      <c r="G151" s="2">
+        <v>41548</v>
+      </c>
+      <c r="H151" s="2">
+        <v>41548</v>
+      </c>
+      <c r="I151">
+        <v>1</v>
+      </c>
+      <c r="J151" s="2">
+        <v>34578</v>
+      </c>
+      <c r="K151" s="2" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>281</v>
       </c>
+      <c r="B152">
+        <v>1</v>
+      </c>
       <c r="C152">
         <v>35.398029999999999</v>
       </c>
       <c r="D152">
         <v>-118.91293</v>
       </c>
-      <c r="G152" s="2"/>
+      <c r="E152">
+        <v>5</v>
+      </c>
+      <c r="F152">
+        <v>15</v>
+      </c>
+      <c r="G152" s="2">
+        <v>41334</v>
+      </c>
       <c r="H152" s="2"/>
-      <c r="J152" s="2"/>
-      <c r="K152" s="2"/>
+      <c r="I152">
+        <v>0</v>
+      </c>
+      <c r="J152" s="2">
+        <v>33848</v>
+      </c>
+      <c r="K152" s="2" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>282</v>
       </c>
+      <c r="B153">
+        <v>1</v>
+      </c>
       <c r="C153">
         <v>35.531619999999997</v>
       </c>
       <c r="D153">
         <v>-82.842309999999998</v>
       </c>
-      <c r="G153" s="2"/>
-      <c r="H153" s="2"/>
-      <c r="J153" s="2"/>
+      <c r="E153">
+        <v>5</v>
+      </c>
+      <c r="F153">
+        <v>0.1</v>
+      </c>
+      <c r="G153" s="2">
+        <v>41334</v>
+      </c>
+      <c r="H153" s="2">
+        <v>41334</v>
+      </c>
+      <c r="I153">
+        <v>1</v>
+      </c>
+      <c r="J153" s="2">
+        <v>34759</v>
+      </c>
+      <c r="K153" s="2" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>283</v>
       </c>
+      <c r="B154">
+        <v>1</v>
+      </c>
       <c r="C154">
         <v>37.207470000000001</v>
       </c>
       <c r="D154">
         <v>-120.35635000000001</v>
       </c>
-      <c r="G154" s="2"/>
+      <c r="E154">
+        <v>4</v>
+      </c>
+      <c r="G154" s="2">
+        <v>41122</v>
+      </c>
       <c r="H154" s="2"/>
-      <c r="J154" s="2"/>
+      <c r="I154">
+        <v>0</v>
+      </c>
+      <c r="J154" s="2">
+        <v>36008</v>
+      </c>
+      <c r="K154" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="L154" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>284</v>
       </c>
+      <c r="B155">
+        <v>0</v>
+      </c>
       <c r="C155">
         <v>27.470079999999999</v>
       </c>
@@ -6332,26 +6580,59 @@
       </c>
       <c r="G155" s="2"/>
       <c r="H155" s="2"/>
-      <c r="J155" s="2"/>
+      <c r="I155" t="s">
+        <v>366</v>
+      </c>
+      <c r="J155" s="2">
+        <v>34394</v>
+      </c>
+      <c r="K155" s="2" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>285</v>
       </c>
+      <c r="B156">
+        <v>1</v>
+      </c>
       <c r="C156">
-        <v>27.016660000000002</v>
+        <v>27.018017</v>
       </c>
       <c r="D156">
-        <v>-82.019189999999995</v>
-      </c>
-      <c r="G156" s="2"/>
+        <v>-82.020280999999997</v>
+      </c>
+      <c r="E156">
+        <v>3</v>
+      </c>
+      <c r="F156">
+        <v>2.57</v>
+      </c>
+      <c r="G156" s="2">
+        <v>40513</v>
+      </c>
       <c r="H156" s="2"/>
-      <c r="J156" s="2"/>
+      <c r="I156">
+        <v>0.5</v>
+      </c>
+      <c r="J156" s="2">
+        <v>34731</v>
+      </c>
+      <c r="K156" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="L156" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>286</v>
       </c>
+      <c r="B157">
+        <v>0</v>
+      </c>
       <c r="C157">
         <v>37.360469999999999</v>
       </c>
@@ -6360,7 +6641,12 @@
       </c>
       <c r="G157" s="2"/>
       <c r="H157" s="2"/>
-      <c r="J157" s="2"/>
+      <c r="J157" s="2">
+        <v>34090</v>
+      </c>
+      <c r="K157" s="2" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
@@ -6375,11 +6661,20 @@
       <c r="G158" s="2"/>
       <c r="H158" s="2"/>
       <c r="J158" s="2"/>
+      <c r="K158" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="L158" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>288</v>
       </c>
+      <c r="B159">
+        <v>0</v>
+      </c>
       <c r="C159">
         <v>38.628270000000001</v>
       </c>
@@ -6388,12 +6683,20 @@
       </c>
       <c r="G159" s="2"/>
       <c r="H159" s="2"/>
-      <c r="J159" s="2"/>
+      <c r="J159" s="2">
+        <v>34121</v>
+      </c>
+      <c r="K159" s="2" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>289</v>
       </c>
+      <c r="B160">
+        <v>0</v>
+      </c>
       <c r="C160">
         <v>26.323779999999999</v>
       </c>
@@ -6402,26 +6705,55 @@
       </c>
       <c r="G160" s="2"/>
       <c r="H160" s="2"/>
-      <c r="J160" s="2"/>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J160" s="2">
+        <v>34700</v>
+      </c>
+      <c r="K160" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>290</v>
       </c>
+      <c r="B161">
+        <v>1</v>
+      </c>
       <c r="C161">
         <v>25.802820000000001</v>
       </c>
       <c r="D161">
         <v>-80.124129999999994</v>
       </c>
-      <c r="G161" s="2"/>
-      <c r="H161" s="2"/>
-      <c r="J161" s="2"/>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E161">
+        <v>1</v>
+      </c>
+      <c r="G161" s="2">
+        <v>40603</v>
+      </c>
+      <c r="H161" s="2">
+        <v>40603</v>
+      </c>
+      <c r="I161">
+        <v>1</v>
+      </c>
+      <c r="J161" s="2">
+        <v>34700</v>
+      </c>
+      <c r="K161" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="L161" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>291</v>
       </c>
+      <c r="B162">
+        <v>0</v>
+      </c>
       <c r="C162">
         <v>45.014516</v>
       </c>
@@ -6430,12 +6762,20 @@
       </c>
       <c r="G162" s="2"/>
       <c r="H162" s="2"/>
-      <c r="J162" s="2"/>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J162" s="2">
+        <v>33786</v>
+      </c>
+      <c r="K162" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>292</v>
       </c>
+      <c r="B163">
+        <v>0</v>
+      </c>
       <c r="C163">
         <v>38.683869999999999</v>
       </c>
@@ -6444,12 +6784,20 @@
       </c>
       <c r="G163" s="2"/>
       <c r="H163" s="2"/>
-      <c r="J163" s="2"/>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J163" s="2">
+        <v>34121</v>
+      </c>
+      <c r="K163" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>293</v>
       </c>
+      <c r="B164">
+        <v>0</v>
+      </c>
       <c r="C164">
         <v>36.853920000000002</v>
       </c>
@@ -6458,26 +6806,55 @@
       </c>
       <c r="G164" s="2"/>
       <c r="H164" s="2"/>
-      <c r="J164" s="2"/>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J164" s="2">
+        <v>36008</v>
+      </c>
+      <c r="K164" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>294</v>
       </c>
+      <c r="B165">
+        <v>1</v>
+      </c>
       <c r="C165">
         <v>35.460189999999997</v>
       </c>
       <c r="D165">
         <v>-79.401840000000007</v>
       </c>
-      <c r="G165" s="2"/>
-      <c r="H165" s="2"/>
-      <c r="J165" s="2"/>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E165">
+        <v>3</v>
+      </c>
+      <c r="F165">
+        <v>2</v>
+      </c>
+      <c r="G165" s="2">
+        <v>42278</v>
+      </c>
+      <c r="H165" s="2">
+        <v>42278</v>
+      </c>
+      <c r="I165">
+        <v>1</v>
+      </c>
+      <c r="J165" s="2">
+        <v>34001</v>
+      </c>
+      <c r="K165" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>295</v>
       </c>
+      <c r="B166">
+        <v>0</v>
+      </c>
       <c r="C166">
         <v>34.278399999999998</v>
       </c>
@@ -6486,26 +6863,55 @@
       </c>
       <c r="G166" s="2"/>
       <c r="H166" s="2"/>
-      <c r="J166" s="2"/>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J166" s="2">
+        <v>34455</v>
+      </c>
+      <c r="K166" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>296</v>
       </c>
+      <c r="B167">
+        <v>1</v>
+      </c>
       <c r="C167">
         <v>40.381860000000003</v>
       </c>
       <c r="D167">
         <v>-73.973389999999995</v>
       </c>
-      <c r="G167" s="2"/>
-      <c r="H167" s="2"/>
-      <c r="J167" s="2"/>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E167">
+        <v>1</v>
+      </c>
+      <c r="F167">
+        <v>10</v>
+      </c>
+      <c r="G167" s="2">
+        <v>41518</v>
+      </c>
+      <c r="H167" s="2">
+        <v>41518</v>
+      </c>
+      <c r="I167">
+        <v>1</v>
+      </c>
+      <c r="J167" s="2">
+        <v>34759</v>
+      </c>
+      <c r="K167" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>297</v>
       </c>
+      <c r="B168">
+        <v>0</v>
+      </c>
       <c r="C168">
         <v>39.10566</v>
       </c>
@@ -6514,25 +6920,58 @@
       </c>
       <c r="G168" s="2"/>
       <c r="H168" s="2"/>
-      <c r="J168" s="2"/>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J168" s="2">
+        <v>33298</v>
+      </c>
+      <c r="K168" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="L168" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>298</v>
       </c>
+      <c r="B169">
+        <v>1</v>
+      </c>
       <c r="C169">
         <v>38.485550000000003</v>
       </c>
       <c r="D169">
         <v>-121.55014</v>
       </c>
-      <c r="G169" s="2"/>
-      <c r="H169" s="2"/>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E169">
+        <v>3</v>
+      </c>
+      <c r="G169" s="2">
+        <v>42095</v>
+      </c>
+      <c r="H169" s="2">
+        <v>42095</v>
+      </c>
+      <c r="I169">
+        <v>1</v>
+      </c>
+      <c r="J169" s="2">
+        <v>34121</v>
+      </c>
+      <c r="K169" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="L169" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>299</v>
       </c>
+      <c r="B170">
+        <v>0</v>
+      </c>
       <c r="C170">
         <v>38.343330000000002</v>
       </c>
@@ -6541,8 +6980,17 @@
       </c>
       <c r="G170" s="2"/>
       <c r="H170" s="2"/>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J170" s="2">
+        <v>34151</v>
+      </c>
+      <c r="K170" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="L170" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>300</v>
       </c>
@@ -6554,76 +7002,202 @@
       </c>
       <c r="G171" s="2"/>
       <c r="H171" s="2"/>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J171" s="2">
+        <v>34731</v>
+      </c>
+      <c r="K171" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="L171" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>301</v>
       </c>
+      <c r="B172">
+        <v>0.5</v>
+      </c>
       <c r="C172">
-        <v>41.279989999999998</v>
+        <v>41.260330000000003</v>
       </c>
       <c r="D172">
-        <v>-121.87784000000001</v>
-      </c>
-      <c r="G172" s="2"/>
-      <c r="H172" s="2"/>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
+        <v>-121.92778</v>
+      </c>
+      <c r="E172">
+        <v>1</v>
+      </c>
+      <c r="F172">
+        <v>80.5</v>
+      </c>
+      <c r="G172" s="2">
+        <v>41821</v>
+      </c>
+      <c r="H172" s="2">
+        <v>41821</v>
+      </c>
+      <c r="I172">
+        <v>1</v>
+      </c>
+      <c r="J172" s="2">
+        <v>34182</v>
+      </c>
+      <c r="K172" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="L172" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>302</v>
       </c>
+      <c r="B173">
+        <v>0.5</v>
+      </c>
       <c r="C173">
         <v>47.364310000000003</v>
       </c>
       <c r="D173">
         <v>-124.07126</v>
       </c>
-      <c r="G173" s="2"/>
-      <c r="H173" s="2"/>
-    </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E173">
+        <v>3</v>
+      </c>
+      <c r="F173">
+        <v>40</v>
+      </c>
+      <c r="G173" s="2">
+        <v>39873</v>
+      </c>
+      <c r="H173" s="2">
+        <v>39873</v>
+      </c>
+      <c r="I173">
+        <v>1</v>
+      </c>
+      <c r="J173" s="2">
+        <v>34516</v>
+      </c>
+      <c r="K173" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>303</v>
       </c>
+      <c r="B174">
+        <v>0.5</v>
+      </c>
       <c r="C174">
         <v>37.280230000000003</v>
       </c>
       <c r="D174">
         <v>-76.012810000000002</v>
       </c>
-      <c r="G174" s="2"/>
-      <c r="H174" s="2"/>
-    </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E174">
+        <v>3</v>
+      </c>
+      <c r="F174">
+        <v>3.3</v>
+      </c>
+      <c r="G174" s="2">
+        <v>41334</v>
+      </c>
+      <c r="H174" s="2">
+        <v>41334</v>
+      </c>
+      <c r="I174">
+        <v>0.5</v>
+      </c>
+      <c r="J174" s="2">
+        <v>34394</v>
+      </c>
+      <c r="K174" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="L174" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>304</v>
       </c>
+      <c r="B175">
+        <v>1</v>
+      </c>
       <c r="C175">
-        <v>39.737819999999999</v>
+        <v>39.738871000000003</v>
       </c>
       <c r="D175">
-        <v>-121.81973000000001</v>
-      </c>
-      <c r="G175" s="2"/>
-      <c r="H175" s="2"/>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
+        <v>-121.822782</v>
+      </c>
+      <c r="E175">
+        <v>3</v>
+      </c>
+      <c r="F175">
+        <v>0.8</v>
+      </c>
+      <c r="G175" s="2">
+        <v>41395</v>
+      </c>
+      <c r="H175" s="2">
+        <v>42095</v>
+      </c>
+      <c r="I175">
+        <v>1</v>
+      </c>
+      <c r="J175" s="2">
+        <v>36008</v>
+      </c>
+      <c r="K175" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>305</v>
       </c>
+      <c r="B176">
+        <v>1</v>
+      </c>
       <c r="C176">
         <v>27.163499999999999</v>
       </c>
       <c r="D176">
         <v>-82.43047</v>
       </c>
-      <c r="G176" s="2"/>
+      <c r="E176">
+        <v>3</v>
+      </c>
+      <c r="F176">
+        <v>27</v>
+      </c>
+      <c r="G176" s="2">
+        <v>40513</v>
+      </c>
       <c r="H176" s="2"/>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I176">
+        <v>0</v>
+      </c>
+      <c r="J176" s="2">
+        <v>34700</v>
+      </c>
+      <c r="K176" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>306</v>
       </c>
+      <c r="B177">
+        <v>0</v>
+      </c>
       <c r="C177">
         <v>44.387390000000003</v>
       </c>
@@ -6632,11 +7206,20 @@
       </c>
       <c r="G177" s="2"/>
       <c r="H177" s="2"/>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J177" s="2">
+        <v>36008</v>
+      </c>
+      <c r="K177" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>307</v>
       </c>
+      <c r="B178">
+        <v>0</v>
+      </c>
       <c r="C178">
         <v>38.300789999999999</v>
       </c>
@@ -6645,11 +7228,20 @@
       </c>
       <c r="G178" s="2"/>
       <c r="H178" s="2"/>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J178" s="2">
+        <v>34121</v>
+      </c>
+      <c r="K178" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>308</v>
       </c>
+      <c r="B179">
+        <v>0</v>
+      </c>
       <c r="C179">
         <v>40.361719999999998</v>
       </c>
@@ -6658,11 +7250,23 @@
       </c>
       <c r="G179" s="2"/>
       <c r="H179" s="2"/>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J179" s="2">
+        <v>36039</v>
+      </c>
+      <c r="K179" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L179" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>309</v>
       </c>
+      <c r="B180">
+        <v>0</v>
+      </c>
       <c r="C180">
         <v>37.757510000000003</v>
       </c>
@@ -6671,24 +7275,55 @@
       </c>
       <c r="G180" s="2"/>
       <c r="H180" s="2"/>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J180" s="2">
+        <v>14580</v>
+      </c>
+      <c r="K180" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>310</v>
       </c>
+      <c r="B181">
+        <v>1</v>
+      </c>
       <c r="C181">
         <v>38.403570000000002</v>
       </c>
       <c r="D181">
         <v>-122.81506</v>
       </c>
-      <c r="G181" s="2"/>
-      <c r="H181" s="2"/>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E181">
+        <v>5</v>
+      </c>
+      <c r="F181">
+        <v>0.06</v>
+      </c>
+      <c r="G181" s="2">
+        <v>40725</v>
+      </c>
+      <c r="H181" s="2">
+        <v>40725</v>
+      </c>
+      <c r="I181">
+        <v>1</v>
+      </c>
+      <c r="J181" s="2">
+        <v>34151</v>
+      </c>
+      <c r="K181" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>311</v>
       </c>
+      <c r="B182">
+        <v>0</v>
+      </c>
       <c r="C182">
         <v>34.750680000000003</v>
       </c>
@@ -6697,11 +7332,20 @@
       </c>
       <c r="G182" s="2"/>
       <c r="H182" s="2"/>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J182" s="2">
+        <v>34578</v>
+      </c>
+      <c r="K182" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>312</v>
       </c>
+      <c r="B183">
+        <v>0</v>
+      </c>
       <c r="C183">
         <v>34.729520000000001</v>
       </c>
@@ -6710,40 +7354,46 @@
       </c>
       <c r="G183" s="2"/>
       <c r="H183" s="2"/>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J183" s="2">
+        <v>34578</v>
+      </c>
+      <c r="K183" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G184" s="2"/>
       <c r="H184" s="2"/>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G185" s="2"/>
       <c r="H185" s="2"/>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G186" s="2"/>
       <c r="H186" s="2"/>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G187" s="2"/>
       <c r="H187" s="2"/>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G188" s="2"/>
       <c r="H188" s="2"/>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G189" s="2"/>
       <c r="H189" s="2"/>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G190" s="2"/>
       <c r="H190" s="2"/>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G191" s="2"/>
       <c r="H191" s="2"/>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G192" s="2"/>
       <c r="H192" s="2"/>
     </row>

</xml_diff>